<commit_message>
Descriptive complete along with comments
</commit_message>
<xml_diff>
--- a/Appendices.xlsx
+++ b/Appendices.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="171">
   <si>
     <t>FIELD</t>
   </si>
@@ -304,15 +304,60 @@
     <t>CHANNEL_CODE</t>
   </si>
   <si>
+    <t>POS type hierarchy level 2 unique identifier</t>
+  </si>
+  <si>
+    <t>CHANNEL_NAME</t>
+  </si>
+  <si>
+    <t>POS type hierarchy level 2 name</t>
+  </si>
+  <si>
     <t>SUB_CHANNEL_CODE</t>
   </si>
   <si>
+    <t>POS type hierarchy level 3 unique identifier</t>
+  </si>
+  <si>
+    <t>SUB_CHANNEL_NAME</t>
+  </si>
+  <si>
+    <t>POS type hierarchy level 3 name</t>
+  </si>
+  <si>
     <t>ELEMENT_CODE</t>
   </si>
   <si>
+    <t>POS type hierarchy level 4 unique identifier</t>
+  </si>
+  <si>
+    <t>ELEMENT_NAME</t>
+  </si>
+  <si>
+    <t>POS type hierarchy level 4 name</t>
+  </si>
+  <si>
     <t>SUB_ELEMENT_CODE</t>
   </si>
   <si>
+    <t>POS type hierarchy level 5 unique identifier</t>
+  </si>
+  <si>
+    <t>SUB_ELEMENT_NAME</t>
+  </si>
+  <si>
+    <t>POS type hierarchy level 5 name</t>
+  </si>
+  <si>
+    <t>SHOPPER_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>OWNER_CODE</t>
+  </si>
+  <si>
+    <t>POS owner unique identifier</t>
+  </si>
+  <si>
     <t>DOC_DATE_YEAR</t>
   </si>
   <si>
@@ -376,9 +421,6 @@
     <t>Urban</t>
   </si>
   <si>
-    <t>CHANNEL_NAME</t>
-  </si>
-  <si>
     <t>Retail</t>
   </si>
   <si>
@@ -389,9 +431,6 @@
   </si>
   <si>
     <t>International Modern Trade</t>
-  </si>
-  <si>
-    <t>SUB_CHANNEL_NAME</t>
   </si>
   <si>
     <t>Grocery</t>
@@ -512,7 +551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -533,11 +572,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -588,7 +622,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,14 +635,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -617,11 +643,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -644,15 +670,14 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="124.464285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,560 +1003,561 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>1</v>
+      <c r="B1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="n">
+      <c r="C10" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D14" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="n">
+      <c r="B18" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="C19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="n">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="n">
+      <c r="D26" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="n">
+      <c r="B28" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <v>11</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <v>13</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <v>14</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <v>17</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="n">
+      <c r="B29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7" t="n">
-        <v>18</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="n">
+      <c r="D31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7" t="n">
-        <v>19</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <v>21</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C23" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>22</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C25" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="7" t="n">
-        <v>24</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="7" t="n">
-        <v>25</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B27" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7" t="n">
-        <v>26</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="C32" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B28" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7" t="n">
-        <v>27</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B29" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>28</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D30" s="7" t="n">
-        <v>29</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C31" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C32" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" s="7" t="n">
-        <v>31</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1550,17 +1576,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -1579,7 +1605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -1587,7 +1613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>77</v>
       </c>
@@ -1595,7 +1621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
@@ -1603,7 +1629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
@@ -1611,7 +1637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
@@ -1619,7 +1645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1627,7 +1653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1643,7 +1669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
@@ -1651,7 +1677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1659,15 +1685,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -1675,15 +1701,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
@@ -1691,7 +1717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1699,7 +1725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1707,7 +1733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>87</v>
       </c>
@@ -1715,7 +1741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>89</v>
       </c>
@@ -1723,84 +1749,148 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1827,9 +1917,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1880,9 +1969,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,7 +1994,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1933,9 +2021,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1959,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1986,14 +2073,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2004,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2039,48 +2125,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>115</v>
+      <c r="B1" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>116</v>
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>117</v>
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>118</v>
+      <c r="B4" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>119</v>
+      <c r="B5" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2100,138 +2187,128 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>120</v>
+      <c r="B1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>121</v>
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>122</v>
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="n">
+      <c r="A4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>123</v>
+      <c r="C4" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="n">
+      <c r="A5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>124</v>
+      <c r="C5" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>117</v>
+      <c r="A6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>125</v>
+      <c r="B7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>126</v>
+      <c r="B8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>127</v>
+      <c r="B9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>117</v>
+      <c r="B10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2253,309 +2330,310 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>1</v>
+      <c r="B1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>129</v>
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>130</v>
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="n">
+      <c r="A4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7" t="n">
+      <c r="B20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="B21" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B21" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>